<commit_message>
Change US from region to country
</commit_message>
<xml_diff>
--- a/source_data/protocols/NCT04573309/NCT04573309.xlsx
+++ b/source_data/protocols/NCT04573309/NCT04573309.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/NCT04573309/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F7B500-1BEC-AB4A-9F3E-266A3D87FE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680531C1-94B9-1242-9AF2-991200F6B004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38140" yWindow="500" windowWidth="36400" windowHeight="19900" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -485,10 +485,10 @@
     <t>scopes</t>
   </si>
   <si>
+    <t>Sponsor Approval Date</t>
+  </si>
+  <si>
     <t>protocol_document</t>
-  </si>
-  <si>
-    <t>Protocol Effective Date</t>
   </si>
   <si>
     <t>Global</t>
@@ -6972,8 +6972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
         <v>1356</v>
@@ -7166,7 +7166,7 @@
         <v>1352</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F17" s="29">
         <v>43963</v>
@@ -7177,7 +7177,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
         <v>1357</v>
@@ -7189,7 +7189,7 @@
         <v>1353</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18" s="29">
         <v>44061</v>
@@ -7200,7 +7200,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B19" t="s">
         <v>1358</v>
@@ -7212,7 +7212,7 @@
         <v>1354</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F19" s="29">
         <v>44274</v>
@@ -7223,7 +7223,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
         <v>1359</v>
@@ -7235,7 +7235,7 @@
         <v>1355</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" s="29">
         <v>44439</v>
@@ -7246,7 +7246,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
         <v>1360</v>
@@ -7258,7 +7258,7 @@
         <v>1366</v>
       </c>
       <c r="E21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F21" s="29">
         <v>44638</v>

</xml_diff>